<commit_message>
fixing lab solution mistake
</commit_message>
<xml_diff>
--- a/03-04-DBFundamentals_MySQL/Day-03/Lab-02-Solution.xlsx
+++ b/03-04-DBFundamentals_MySQL/Day-03/Lab-02-Solution.xlsx
@@ -264,7 +264,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -322,14 +322,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -425,7 +417,7 @@
   <dimension ref="A3:J13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="1" sqref="F17:G19 A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -437,10 +429,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -594,7 +586,7 @@
   <dimension ref="A3:K23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="1" sqref="F17:G19 A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -605,10 +597,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="4.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -812,7 +804,7 @@
   <dimension ref="A3:R13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="1" sqref="F17:G19 A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -823,10 +815,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -974,13 +966,13 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="1" sqref="F17:G19 A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.25"/>
@@ -990,7 +982,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1047,7 +1039,7 @@
       <c r="F2" s="14" t="n">
         <v>405</v>
       </c>
-      <c r="G2" s="15" t="n">
+      <c r="G2" s="14" t="n">
         <v>2000</v>
       </c>
       <c r="H2" s="8" t="n">
@@ -1064,25 +1056,25 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="n">
+      <c r="A3" s="15" t="n">
         <v>1001</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="16" t="n">
+      <c r="D3" s="15" t="n">
         <v>210</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="16" t="n">
+      <c r="F3" s="15" t="n">
         <v>405</v>
       </c>
-      <c r="G3" s="17" t="n">
+      <c r="G3" s="15" t="n">
         <v>2000</v>
       </c>
       <c r="H3" s="9" t="n">
@@ -1099,25 +1091,25 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="n">
+      <c r="A4" s="15" t="n">
         <v>1001</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="16" t="n">
+      <c r="D4" s="15" t="n">
         <v>210</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="16" t="n">
+      <c r="F4" s="15" t="n">
         <v>405</v>
       </c>
-      <c r="G4" s="17" t="n">
+      <c r="G4" s="15" t="n">
         <v>2000</v>
       </c>
       <c r="H4" s="9" t="n">
@@ -1157,7 +1149,7 @@
   <dimension ref="A3:G19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1167,9 +1159,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1251,7 +1243,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
@@ -1263,6 +1255,12 @@
       <c r="E13" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="F13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
@@ -1277,7 +1275,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="3" t="s">
         <v>5</v>
       </c>
@@ -1287,15 +1285,9 @@
       <c r="E16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="18" t="n">
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="16" t="n">
         <v>405</v>
       </c>
       <c r="D17" s="8" t="n">
@@ -1304,15 +1296,11 @@
       <c r="E17" s="8" t="n">
         <v>40</v>
       </c>
-      <c r="F17" s="19" t="n">
-        <v>1001</v>
-      </c>
-      <c r="G17" s="19" t="n">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="18" t="n">
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="16" t="n">
         <v>405</v>
       </c>
       <c r="D18" s="9" t="n">
@@ -1321,15 +1309,11 @@
       <c r="E18" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="F18" s="19" t="n">
-        <v>1001</v>
-      </c>
-      <c r="G18" s="19" t="n">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="18" t="n">
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="16" t="n">
         <v>405</v>
       </c>
       <c r="D19" s="9" t="n">
@@ -1338,12 +1322,8 @@
       <c r="E19" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="F19" s="19" t="n">
-        <v>1001</v>
-      </c>
-      <c r="G19" s="19" t="n">
-        <v>210</v>
-      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>